<commit_message>
added all the 6 projects to the excel file
</commit_message>
<xml_diff>
--- a/site_pages/Projects.xlsx
+++ b/site_pages/Projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Web Development\Website-danishnaseemoid.com\site_pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848D68AC-6A25-4339-8537-C1301F1FAE92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52E52C3-487E-450D-AFEB-00E1D2F1F245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23355" yWindow="4485" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4035" yWindow="5595" windowWidth="38700" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>language</t>
   </si>
@@ -70,13 +70,136 @@
   </si>
   <si>
     <t>../pics/project_cards/Web_Server/Capture5.PNG</t>
+  </si>
+  <si>
+    <t>[../pics/project_cards/Todays_songs/Capture.PNG][../pics/project_cards/Todays_songs/Capture2.PNG][../pics/project_cards/Todays_songs/Capture3.PNG][../pics/project_cards/Todays_songs/Capture4.PNG]</t>
+  </si>
+  <si>
+    <t>[First slide][Second slide][Third slide][Fourth slide]</t>
+  </si>
+  <si>
+    <t>[Lists the songs to the user from two different sites, and prompts them for selection][Opens the selected song number in Chrome browser.][Opens another song selection (after prompting the user whether they want to listen to any other song, and their response being yes) in YouTube.][The program exits with a goodbye response, after the user is done listening to songs.]</t>
+  </si>
+  <si>
+    <t>https://github.com/danishnaseem05/todays_songs</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>fab fa-java</t>
+  </si>
+  <si>
+    <t>Sorted Doubly Linked List</t>
+  </si>
+  <si>
+    <t>This is the GUI representation of my customly implemented Doubly Linked List. This List is Sorted and only allows unique integer values. Furthermore, the GUI is easily navigable and its purpose is to Add an unique integer while keeping the list sorted, Delete an integer if it exists in the list, and Display All integers currently stored within the list. Adding to and displaying an empty list, deleting an unstored integer, or entering a non-integer value; all would display errors.</t>
+  </si>
+  <si>
+    <t>../pics/project_cards/Doubly_Linked_Sorted_List/Capture5.PNG</t>
+  </si>
+  <si>
+    <t>[../pics/project_cards/Doubly_Linked_Sorted_List/Capture.PNG][../pics/project_cards/Doubly_Linked_Sorted_List/Capture2.PNG][../pics/project_cards/Doubly_Linked_Sorted_List/Capture3.PNG][../pics/project_cards/Doubly_Linked_Sorted_List/Capture4.PNG][../pics/project_cards/Doubly_Linked_Sorted_List/Capture5.PNG][../pics/project_cards/Doubly_Linked_Sorted_List/Capture6.PNG][../pics/project_cards/Doubly_Linked_Sorted_List/Capture7.PNG][../pics/project_cards/Doubly_Linked_Sorted_List/Capture8.PNG][../pics/project_cards/Doubly_Linked_Sorted_List/Capture9.PNG][../pics/project_cards/Doubly_Linked_Sorted_List/Capture10.PNG][../pics/project_cards/Doubly_Linked_Sorted_List/Capture11.PNG][../pics/project_cards/Doubly_Linked_Sorted_List/Capture12.PNG]</t>
+  </si>
+  <si>
+    <t>[First slide][Second slide][Third slide][Fourth slide][Fifth slide]</t>
+  </si>
+  <si>
+    <t>[First slide][Second slide][Third slide][Fourth slide][Fifth slide][Sixth slide]</t>
+  </si>
+  <si>
+    <t>[First slide][Second slide][Third slide][Fourth slide][Fifth slide][Sixth slide][Seventh slide][Eight slide][Ninth slide][Tenth slide][Eleventh slide][Twelveth slide]</t>
+  </si>
+  <si>
+    <t>[After launching the app.][Clicked on Display All on without adding first.][Entering number 1500 into the input entry][Confirmation Log of number 1500 being added to the list.][After adding a few items to the list.][After clicking Display All to display all the integers currently stored in the list.][Trying to add or delete without entering a number in the entry box.][Entered a non-integer value.][Deleted number 2, 43, and 754 from the list.][Displaying list after deleting the numbers.][Trying to add an already existant number in the list.][After the removing the last item from the list.]</t>
+  </si>
+  <si>
+    <t>https://github.com/danishnaseem05/Doubly-Linked-Sorted-List</t>
+  </si>
+  <si>
+    <t>Ruby</t>
+  </si>
+  <si>
+    <t>fas fa-gem</t>
+  </si>
+  <si>
+    <t>Today\'s Songs</t>
+  </si>
+  <si>
+    <t>This CLI executable program provides the user with top songs of the day. It collects the song data from two different sites, lists them to the user, and enables them to listen to these songs by opening the user\'s preferred song in the chrome browser.</t>
+  </si>
+  <si>
+    <t>../pics/project_cards/Todays_songs/Capture2.PNG</t>
+  </si>
+  <si>
+    <t>[../pics/project_cards/Web_Server/Capture.PNG][../pics/project_cards/Web_Server/Capture2.PNG][../pics/project_cards/Web_Server/Capture3.PNG][../pics/project_cards/Web_Server/Capture4.PNG][../pics/project_cards/Web_Server/Capture5.PNG]</t>
+  </si>
+  <si>
+    <t>[Started the server on linux in windows.][Ran localhost:8000/tests/html/cars/ford.html in Google Chrome.][Created and saved ford.html inside static/tests/html/cars/ford.html][ford.html file saved inside the path.][Connected two clients (Microsoft Edge and Google Chrome) to the Web Server. Runing localhost:8000/tests/html/cars/ford.html in Chrome, and localhost:8000/tests/html/index.html in Edge.]</t>
+  </si>
+  <si>
+    <t>https://github.com/danishnaseem05/WebServer</t>
+  </si>
+  <si>
+    <t>Wave Worm</t>
+  </si>
+  <si>
+    <t>Video and Sound Encoder</t>
+  </si>
+  <si>
+    <t>CLI Tic Tac Toe</t>
+  </si>
+  <si>
+    <t>Wave Worm is a single player 2D Java game. The user tackles the various worms using keyboard keys, and makes his/her way across levels, while maintaining a top score.</t>
+  </si>
+  <si>
+    <t>../pics/project_cards/Wave_worm/Capture8.PNG</t>
+  </si>
+  <si>
+    <t>../pics/project_cards/Video_and_Sound_Encoder/Capture5.PNG</t>
+  </si>
+  <si>
+    <t>../pics/project_cards/Tic_Tac_Toe/Capture5.PNG</t>
+  </si>
+  <si>
+    <t>This gui program makes bash calls to ffmpeg in order to encode either mov (includes audio encoding from surround to stereo) or dnxhd format video(s), hence condensing their size all the while preserving quality, as well as the directory structure. And this software was made during my time interning for FCB Chicago.</t>
+  </si>
+  <si>
+    <t>This is a CLI version of Tic Tac Toe, providing the user with single player, double player, and even zero player (meaning the player gets to watch computer vs computer) experience.</t>
+  </si>
+  <si>
+    <t>[../pics/project_cards/Wave_worm/Capture.PNG][../pics/project_cards/Wave_worm/Capture2.PNG][../pics/project_cards/Wave_worm/Capture3.PNG][../pics/project_cards/Wave_worm/Capture8.PNG][../pics/project_cards/Wave_worm/Capture6.PNG][../pics/project_cards/Wave_worm/Capture7.PNG]</t>
+  </si>
+  <si>
+    <t>[The main menu screen; having mouse event listeners for the user to easily navigate through with a mouse/touchpad.][The help menu, which is pretty self-explanatory][After pressing Play, the user gets prompt to select a difficulty mode. The Hard mode increments the number of enemies as well as introduces a new one.][Gameplay in Hard Mode. The Player being the white square, and the others being different species of enemies, including the green smart enemy, which follows the player.][The final level of the game, where the user comes face to face with the big boss, and his minions.][Like any other 2D game, if your health becomes zero, you loose, and hence comes the game over screen.]</t>
+  </si>
+  <si>
+    <t>https://github.com/danishnaseem05/Wave-Worm-Java-Game</t>
+  </si>
+  <si>
+    <t>[../pics/project_cards/Video_and_Sound_Encoder/Capture.PNG][../pics/project_cards/Video_and_Sound_Encoder/Capture2.PNG][../pics/project_cards/Video_and_Sound_Encoder/Capture3.PNG][../pics/project_cards/Video_and_Sound_Encoder/Capture4.PNG][../pics/project_cards/Video_and_Sound_Encoder/Capture5.PNG]</t>
+  </si>
+  <si>
+    <t>[The main menu of the GUI, giving the user the options of picking from either MOV or DNXHD Encoding.][After selection, it prompts the user to select the input directory containing all the video files. Even if the directory contains any other files, the program would simply just ignore them, and go for the required files.][Warns the user in case of accidental cancellation.][Well, this one I thought would be funny if the user were to accidentally hit cancel and then click on 'No' that they do not wish to exit the program. The program would then respond with a random goofy message.][After the user stops goofing around, *pun intended* the program runs the main ffmpeg conversion using the bash command pipelined from within python]</t>
+  </si>
+  <si>
+    <t>https://github.com/danishnaseem05/Video-and-Sound-Encoder-made-at-FCB</t>
+  </si>
+  <si>
+    <t>[../pics/project_cards/Tic_Tac_Toe/Capture.PNG][../pics/project_cards/Tic_Tac_Toe/Capture2.PNG][../pics/project_cards/Tic_Tac_Toe/Capture3.PNG][../pics/project_cards/Tic_Tac_Toe/Capture6.PNG]</t>
+  </si>
+  <si>
+    <t>[After execution, it greets and then prompts the user for the type of game they'd wish to play.][Here I've chosen a one player game. The game launches with a blank board and is waiting on me to make a move.][A few turns into the game of me vs the computer.][The game ends up in being a draw. It also congragulates the winner with their token name (X or O) if either of the players have won.]</t>
+  </si>
+  <si>
+    <t>https://github.com/danishnaseem05/CLI-Tic-Tac-Toe-Ruby</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +211,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,10 +241,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -124,8 +256,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -404,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,17 +554,17 @@
     <col min="1" max="1" width="7.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="38.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="25.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="48" style="1" customWidth="1"/>
     <col min="10" max="10" width="22.140625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -457,7 +596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -476,9 +615,189 @@
       <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{8ABCA5E3-6B08-4366-835D-BB0F21328BDA}"/>
+    <hyperlink ref="J4" r:id="rId2" xr:uid="{769743E8-DB4E-4850-94F7-2FEECD1C2CD6}"/>
+    <hyperlink ref="J2" r:id="rId3" xr:uid="{44C8D3D2-F095-4BF2-9C7D-45E73EED6EB2}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{ECB9C285-A893-4065-8CAC-482B2BFCB469}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{B07FC93A-CC05-4ADB-8417-8321E68D7685}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{6F7346E5-4FCB-46A5-98FF-B2A2200E8BA5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>